<commit_message>
API and Kubernetes yamls defined
</commit_message>
<xml_diff>
--- a/docs/testing-template.xlsx
+++ b/docs/testing-template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\godoku\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF5DDFB4-9523-4703-B29F-6881828FD3AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0E6F91D-FDE3-42D1-A91B-89E26E8EC197}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1740" yWindow="5580" windowWidth="34560" windowHeight="18324" xr2:uid="{66A231C3-6AEB-44CD-8647-C3A2A8AA17EA}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="25416" xr2:uid="{66A231C3-6AEB-44CD-8647-C3A2A8AA17EA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -597,8 +597,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBFD22E2-2586-466F-8664-1CA732CC441C}">
   <dimension ref="B1:T63"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="Y16" sqref="Y16"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="AF25" sqref="AF25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.109375" defaultRowHeight="25.2" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -621,1323 +621,1323 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="F2" s="4">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="F2" s="4">
+      <c r="G2" s="5">
         <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="G2" s="5" t="str">
+        <v>1</v>
+      </c>
+      <c r="H2" s="11">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="H2" s="11" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+        <v>5</v>
       </c>
       <c r="I2" s="12">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="J2" s="13" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="L2" s="11">
-        <f>IF(B33&lt;&gt;"_",B33, "")</f>
+        <f t="shared" ref="L2:L10" si="1">IF(B33&lt;&gt;"_",B33, "")</f>
         <v>7</v>
       </c>
       <c r="M2" s="12" t="str">
-        <f>IF(C33&lt;&gt;"_",C33, "")</f>
+        <f t="shared" ref="M2:M10" si="2">IF(C33&lt;&gt;"_",C33, "")</f>
         <v/>
       </c>
       <c r="N2" s="13" t="str">
-        <f>IF(D33&lt;&gt;"_",D33, "")</f>
+        <f t="shared" ref="N2:N10" si="3">IF(D33&lt;&gt;"_",D33, "")</f>
         <v/>
       </c>
       <c r="O2" s="3">
-        <f>IF(E33&lt;&gt;"_",E33, "")</f>
+        <f t="shared" ref="O2:O10" si="4">IF(E33&lt;&gt;"_",E33, "")</f>
         <v>2</v>
       </c>
       <c r="P2" s="4">
-        <f>IF(F33&lt;&gt;"_",F33, "")</f>
+        <f t="shared" ref="P2:P10" si="5">IF(F33&lt;&gt;"_",F33, "")</f>
         <v>3</v>
       </c>
       <c r="Q2" s="5">
-        <f>IF(G33&lt;&gt;"_",G33, "")</f>
+        <f t="shared" ref="Q2:Q10" si="6">IF(G33&lt;&gt;"_",G33, "")</f>
         <v>5</v>
       </c>
       <c r="R2" s="11">
-        <f>IF(H33&lt;&gt;"_",H33, "")</f>
+        <f t="shared" ref="R2:R10" si="7">IF(H33&lt;&gt;"_",H33, "")</f>
         <v>9</v>
       </c>
       <c r="S2" s="12" t="str">
-        <f>IF(I33&lt;&gt;"_",I33, "")</f>
+        <f t="shared" ref="S2:S10" si="8">IF(I33&lt;&gt;"_",I33, "")</f>
         <v/>
       </c>
       <c r="T2" s="13" t="str">
-        <f>IF(J33&lt;&gt;"_",J33, "")</f>
+        <f t="shared" ref="T2:T10" si="9">IF(J33&lt;&gt;"_",J33, "")</f>
         <v/>
       </c>
     </row>
     <row r="3" spans="2:20" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="14">
-        <f t="shared" ref="B3:J3" si="1">IF(B23&lt;&gt;"_", B23, "")</f>
+        <f t="shared" ref="B3:J3" si="10">IF(B23&lt;&gt;"_", B23, "")</f>
         <v>3</v>
       </c>
-      <c r="C3" s="15" t="str">
+      <c r="C3" s="15">
+        <f t="shared" si="10"/>
+        <v>5</v>
+      </c>
+      <c r="D3" s="16" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="E3" s="6" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="F3" s="2" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="G3" s="7" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="H3" s="14">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="I3" s="15" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="J3" s="16" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="L3" s="14" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="D3" s="16" t="str">
+      <c r="M3" s="15">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="N3" s="16">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="O3" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="P3" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="Q3" s="7" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="R3" s="14" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="S3" s="15" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="T3" s="16">
+        <f t="shared" si="9"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="2:20" ht="25.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="17" t="str">
+        <f t="shared" ref="B4:J4" si="11">IF(B24&lt;&gt;"_", B24, "")</f>
+        <v/>
+      </c>
+      <c r="C4" s="18" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+      <c r="D4" s="19">
+        <f t="shared" si="11"/>
+        <v>4</v>
+      </c>
+      <c r="E4" s="8" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+      <c r="F4" s="9">
+        <f t="shared" si="11"/>
+        <v>5</v>
+      </c>
+      <c r="G4" s="10">
+        <f t="shared" si="11"/>
+        <v>6</v>
+      </c>
+      <c r="H4" s="17" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+      <c r="I4" s="18" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+      <c r="J4" s="19">
+        <f t="shared" si="11"/>
+        <v>2</v>
+      </c>
+      <c r="L4" s="17" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="E3" s="6" t="str">
+      <c r="M4" s="18">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="N4" s="19" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="O4" s="8" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="P4" s="9" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="Q4" s="10">
+        <f t="shared" si="6"/>
+        <v>6</v>
+      </c>
+      <c r="R4" s="17">
+        <f t="shared" si="7"/>
+        <v>8</v>
+      </c>
+      <c r="S4" s="18" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="T4" s="19">
+        <f t="shared" si="9"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="2:20" ht="25.2" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="3">
+        <f t="shared" ref="B5:J5" si="12">IF(B25&lt;&gt;"_", B25, "")</f>
+        <v>4</v>
+      </c>
+      <c r="C5" s="4">
+        <f t="shared" si="12"/>
+        <v>2</v>
+      </c>
+      <c r="D5" s="5" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+      <c r="E5" s="11">
+        <f t="shared" si="12"/>
+        <v>9</v>
+      </c>
+      <c r="F5" s="12">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="G5" s="13" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+      <c r="H5" s="3" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+      <c r="I5" s="4">
+        <f t="shared" si="12"/>
+        <v>5</v>
+      </c>
+      <c r="J5" s="5" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+      <c r="L5" s="3" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="F3" s="2">
+      <c r="M5" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="N5" s="5">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+      <c r="O5" s="11">
+        <f t="shared" si="4"/>
+        <v>9</v>
+      </c>
+      <c r="P5" s="12" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="Q5" s="13" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="R5" s="3" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="S5" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="T5" s="5" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+    </row>
+    <row r="6" spans="2:20" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="6">
+        <f t="shared" ref="B6:J6" si="13">IF(B26&lt;&gt;"_", B26, "")</f>
+        <v>5</v>
+      </c>
+      <c r="C6" s="2" t="str">
+        <f t="shared" si="13"/>
+        <v/>
+      </c>
+      <c r="D6" s="7" t="str">
+        <f t="shared" si="13"/>
+        <v/>
+      </c>
+      <c r="E6" s="14" t="str">
+        <f t="shared" si="13"/>
+        <v/>
+      </c>
+      <c r="F6" s="15">
+        <f t="shared" si="13"/>
+        <v>6</v>
+      </c>
+      <c r="G6" s="16" t="str">
+        <f t="shared" si="13"/>
+        <v/>
+      </c>
+      <c r="H6" s="6">
+        <f t="shared" si="13"/>
+        <v>8</v>
+      </c>
+      <c r="I6" s="2">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+      <c r="J6" s="7" t="str">
+        <f t="shared" si="13"/>
+        <v/>
+      </c>
+      <c r="L6" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-      <c r="G3" s="7" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="H3" s="14">
-        <f t="shared" si="1"/>
-        <v>7</v>
-      </c>
-      <c r="I3" s="15" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="J3" s="16" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="L3" s="14" t="str">
-        <f>IF(B34&lt;&gt;"_",B34, "")</f>
-        <v/>
-      </c>
-      <c r="M3" s="15">
-        <f>IF(C34&lt;&gt;"_",C34, "")</f>
-        <v>6</v>
-      </c>
-      <c r="N3" s="16">
-        <f>IF(D34&lt;&gt;"_",D34, "")</f>
-        <v>5</v>
-      </c>
-      <c r="O3" s="6" t="str">
-        <f>IF(E34&lt;&gt;"_",E34, "")</f>
-        <v/>
-      </c>
-      <c r="P3" s="2" t="str">
-        <f>IF(F34&lt;&gt;"_",F34, "")</f>
-        <v/>
-      </c>
-      <c r="Q3" s="7" t="str">
-        <f>IF(G34&lt;&gt;"_",G34, "")</f>
-        <v/>
-      </c>
-      <c r="R3" s="14" t="str">
-        <f>IF(H34&lt;&gt;"_",H34, "")</f>
-        <v/>
-      </c>
-      <c r="S3" s="15" t="str">
-        <f>IF(I34&lt;&gt;"_",I34, "")</f>
-        <v/>
-      </c>
-      <c r="T3" s="16">
-        <f>IF(J34&lt;&gt;"_",J34, "")</f>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="2:20" ht="25.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="17">
-        <f t="shared" ref="B4:J4" si="2">IF(B24&lt;&gt;"_", B24, "")</f>
-        <v>8</v>
-      </c>
-      <c r="C4" s="18" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="D4" s="19">
-        <f t="shared" si="2"/>
-        <v>6</v>
-      </c>
-      <c r="E4" s="8" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="F4" s="9">
+        <v/>
+      </c>
+      <c r="M6" s="2">
         <f t="shared" si="2"/>
         <v>7</v>
       </c>
-      <c r="G4" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="H4" s="17">
-        <f t="shared" si="2"/>
-        <v>4</v>
-      </c>
-      <c r="I4" s="18" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="J4" s="19" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="L4" s="17" t="str">
-        <f>IF(B35&lt;&gt;"_",B35, "")</f>
-        <v/>
-      </c>
-      <c r="M4" s="18">
-        <f>IF(C35&lt;&gt;"_",C35, "")</f>
-        <v>9</v>
-      </c>
-      <c r="N4" s="19" t="str">
-        <f>IF(D35&lt;&gt;"_",D35, "")</f>
-        <v/>
-      </c>
-      <c r="O4" s="8" t="str">
-        <f>IF(E35&lt;&gt;"_",E35, "")</f>
-        <v/>
-      </c>
-      <c r="P4" s="9" t="str">
-        <f>IF(F35&lt;&gt;"_",F35, "")</f>
-        <v/>
-      </c>
-      <c r="Q4" s="10">
-        <f>IF(G35&lt;&gt;"_",G35, "")</f>
-        <v>6</v>
-      </c>
-      <c r="R4" s="17">
-        <f>IF(H35&lt;&gt;"_",H35, "")</f>
-        <v>8</v>
-      </c>
-      <c r="S4" s="18" t="str">
-        <f>IF(I35&lt;&gt;"_",I35, "")</f>
-        <v/>
-      </c>
-      <c r="T4" s="19">
-        <f>IF(J35&lt;&gt;"_",J35, "")</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="2:20" ht="25.2" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="3">
-        <f t="shared" ref="B5:J5" si="3">IF(B25&lt;&gt;"_", B25, "")</f>
-        <v>9</v>
-      </c>
-      <c r="C5" s="4" t="str">
+      <c r="N6" s="7" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="D5" s="5">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="E5" s="11" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="F5" s="12" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="G5" s="13" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="H5" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="I5" s="4">
-        <f t="shared" si="3"/>
-        <v>4</v>
-      </c>
-      <c r="J5" s="5" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="L5" s="3" t="str">
-        <f>IF(B36&lt;&gt;"_",B36, "")</f>
-        <v/>
-      </c>
-      <c r="M5" s="4" t="str">
-        <f>IF(C36&lt;&gt;"_",C36, "")</f>
-        <v/>
-      </c>
-      <c r="N5" s="5">
-        <f>IF(D36&lt;&gt;"_",D36, "")</f>
-        <v>8</v>
-      </c>
-      <c r="O5" s="11">
-        <f>IF(E36&lt;&gt;"_",E36, "")</f>
-        <v>9</v>
-      </c>
-      <c r="P5" s="12" t="str">
-        <f>IF(F36&lt;&gt;"_",F36, "")</f>
-        <v/>
-      </c>
-      <c r="Q5" s="13" t="str">
-        <f>IF(G36&lt;&gt;"_",G36, "")</f>
-        <v/>
-      </c>
-      <c r="R5" s="3" t="str">
-        <f>IF(H36&lt;&gt;"_",H36, "")</f>
-        <v/>
-      </c>
-      <c r="S5" s="4" t="str">
-        <f>IF(I36&lt;&gt;"_",I36, "")</f>
-        <v/>
-      </c>
-      <c r="T5" s="5" t="str">
-        <f>IF(J36&lt;&gt;"_",J36, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="6" spans="2:20" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="6">
-        <f t="shared" ref="B6:J6" si="4">IF(B26&lt;&gt;"_", B26, "")</f>
-        <v>6</v>
-      </c>
-      <c r="C6" s="2" t="str">
+      <c r="O6" s="14">
         <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="D6" s="7" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="E6" s="14">
-        <f t="shared" si="4"/>
-        <v>3</v>
-      </c>
-      <c r="F6" s="15" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="G6" s="16" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="H6" s="6" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="I6" s="2">
-        <f t="shared" si="4"/>
-        <v>5</v>
-      </c>
-      <c r="J6" s="7">
-        <f t="shared" si="4"/>
-        <v>7</v>
-      </c>
-      <c r="L6" s="6" t="str">
-        <f>IF(B37&lt;&gt;"_",B37, "")</f>
-        <v/>
-      </c>
-      <c r="M6" s="2">
-        <f>IF(C37&lt;&gt;"_",C37, "")</f>
-        <v>7</v>
-      </c>
-      <c r="N6" s="7" t="str">
-        <f>IF(D37&lt;&gt;"_",D37, "")</f>
-        <v/>
-      </c>
-      <c r="O6" s="14">
-        <f>IF(E37&lt;&gt;"_",E37, "")</f>
         <v>1</v>
       </c>
       <c r="P6" s="15" t="str">
-        <f>IF(F37&lt;&gt;"_",F37, "")</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="Q6" s="16" t="str">
-        <f>IF(G37&lt;&gt;"_",G37, "")</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="R6" s="6" t="str">
-        <f>IF(H37&lt;&gt;"_",H37, "")</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="S6" s="2" t="str">
-        <f>IF(I37&lt;&gt;"_",I37, "")</f>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="T6" s="7">
-        <f>IF(J37&lt;&gt;"_",J37, "")</f>
+        <f t="shared" si="9"/>
         <v>3</v>
       </c>
     </row>
     <row r="7" spans="2:20" ht="25.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="8" t="str">
-        <f t="shared" ref="B7:J7" si="5">IF(B27&lt;&gt;"_", B27, "")</f>
+        <f t="shared" ref="B7:J7" si="14">IF(B27&lt;&gt;"_", B27, "")</f>
         <v/>
       </c>
       <c r="C7" s="9" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="14"/>
         <v/>
       </c>
       <c r="D7" s="10">
-        <f t="shared" si="5"/>
-        <v>5</v>
-      </c>
-      <c r="E7" s="17">
-        <f t="shared" si="5"/>
-        <v>6</v>
-      </c>
-      <c r="F7" s="18">
-        <f t="shared" si="5"/>
-        <v>8</v>
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+      <c r="E7" s="17" t="str">
+        <f t="shared" si="14"/>
+        <v/>
+      </c>
+      <c r="F7" s="18" t="str">
+        <f t="shared" si="14"/>
+        <v/>
       </c>
       <c r="G7" s="19">
+        <f t="shared" si="14"/>
+        <v>5</v>
+      </c>
+      <c r="H7" s="8" t="str">
+        <f t="shared" si="14"/>
+        <v/>
+      </c>
+      <c r="I7" s="9">
+        <f t="shared" si="14"/>
+        <v>2</v>
+      </c>
+      <c r="J7" s="10" t="str">
+        <f t="shared" si="14"/>
+        <v/>
+      </c>
+      <c r="L7" s="8">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="M7" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="N7" s="10">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="O7" s="17" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="P7" s="18">
         <f t="shared" si="5"/>
         <v>4</v>
       </c>
-      <c r="H7" s="8" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="I7" s="9">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-      <c r="J7" s="10" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="L7" s="8">
-        <f>IF(B38&lt;&gt;"_",B38, "")</f>
-        <v>3</v>
-      </c>
-      <c r="M7" s="9" t="str">
-        <f>IF(C38&lt;&gt;"_",C38, "")</f>
-        <v/>
-      </c>
-      <c r="N7" s="10">
-        <f>IF(D38&lt;&gt;"_",D38, "")</f>
-        <v>2</v>
-      </c>
-      <c r="O7" s="17" t="str">
-        <f>IF(E38&lt;&gt;"_",E38, "")</f>
-        <v/>
-      </c>
-      <c r="P7" s="18">
-        <f>IF(F38&lt;&gt;"_",F38, "")</f>
-        <v>4</v>
-      </c>
       <c r="Q7" s="19">
-        <f>IF(G38&lt;&gt;"_",G38, "")</f>
-        <v>7</v>
-      </c>
-      <c r="R7" s="8">
-        <f>IF(H38&lt;&gt;"_",H38, "")</f>
-        <v>6</v>
-      </c>
-      <c r="S7" s="9">
-        <f>IF(I38&lt;&gt;"_",I38, "")</f>
-        <v>8</v>
-      </c>
-      <c r="T7" s="10">
-        <f>IF(J38&lt;&gt;"_",J38, "")</f>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="2:20" ht="25.2" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="11" t="str">
-        <f t="shared" ref="B8:J8" si="6">IF(B28&lt;&gt;"_", B28, "")</f>
-        <v/>
-      </c>
-      <c r="C8" s="12" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="D8" s="13" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="E8" s="3" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="F8" s="4" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="G8" s="5">
         <f t="shared" si="6"/>
         <v>7</v>
       </c>
-      <c r="H8" s="11" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="I8" s="12" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="J8" s="13">
-        <f t="shared" si="6"/>
-        <v>2</v>
-      </c>
-      <c r="L8" s="11" t="str">
-        <f>IF(B39&lt;&gt;"_",B39, "")</f>
-        <v/>
-      </c>
-      <c r="M8" s="12">
-        <f>IF(C39&lt;&gt;"_",C39, "")</f>
-        <v>5</v>
-      </c>
-      <c r="N8" s="13" t="str">
-        <f>IF(D39&lt;&gt;"_",D39, "")</f>
-        <v/>
-      </c>
-      <c r="O8" s="3" t="str">
-        <f>IF(E39&lt;&gt;"_",E39, "")</f>
-        <v/>
-      </c>
-      <c r="P8" s="4">
-        <f>IF(F39&lt;&gt;"_",F39, "")</f>
-        <v>2</v>
-      </c>
-      <c r="Q8" s="5">
-        <f>IF(G39&lt;&gt;"_",G39, "")</f>
-        <v>9</v>
-      </c>
-      <c r="R8" s="11" t="str">
-        <f>IF(H39&lt;&gt;"_",H39, "")</f>
-        <v/>
-      </c>
-      <c r="S8" s="12" t="str">
-        <f>IF(I39&lt;&gt;"_",I39, "")</f>
-        <v/>
-      </c>
-      <c r="T8" s="13" t="str">
-        <f>IF(J39&lt;&gt;"_",J39, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="9" spans="2:20" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="14">
-        <f t="shared" ref="B9:J9" si="7">IF(B29&lt;&gt;"_", B29, "")</f>
-        <v>4</v>
-      </c>
-      <c r="C9" s="15" t="str">
+      <c r="R7" s="8">
         <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="D9" s="16">
-        <f t="shared" si="7"/>
-        <v>9</v>
-      </c>
-      <c r="E9" s="6" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="F9" s="2">
-        <f t="shared" si="7"/>
-        <v>3</v>
-      </c>
-      <c r="G9" s="7" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="H9" s="14">
-        <f t="shared" si="7"/>
-        <v>5</v>
-      </c>
-      <c r="I9" s="15">
-        <f t="shared" si="7"/>
-        <v>7</v>
-      </c>
-      <c r="J9" s="16">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="L9" s="14">
-        <f>IF(B40&lt;&gt;"_",B40, "")</f>
-        <v>6</v>
-      </c>
-      <c r="M9" s="15">
-        <f>IF(C40&lt;&gt;"_",C40, "")</f>
-        <v>3</v>
-      </c>
-      <c r="N9" s="16" t="str">
-        <f>IF(D40&lt;&gt;"_",D40, "")</f>
-        <v/>
-      </c>
-      <c r="O9" s="6" t="str">
-        <f>IF(E40&lt;&gt;"_",E40, "")</f>
-        <v/>
-      </c>
-      <c r="P9" s="2" t="str">
-        <f>IF(F40&lt;&gt;"_",F40, "")</f>
-        <v/>
-      </c>
-      <c r="Q9" s="7" t="str">
-        <f>IF(G40&lt;&gt;"_",G40, "")</f>
-        <v/>
-      </c>
-      <c r="R9" s="14">
-        <f>IF(H40&lt;&gt;"_",H40, "")</f>
-        <v>1</v>
-      </c>
-      <c r="S9" s="15" t="str">
-        <f>IF(I40&lt;&gt;"_",I40, "")</f>
-        <v/>
-      </c>
-      <c r="T9" s="16" t="str">
-        <f>IF(J40&lt;&gt;"_",J40, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="10" spans="2:20" ht="25.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="17">
-        <f t="shared" ref="B10:J10" si="8">IF(B30&lt;&gt;"_", B30, "")</f>
-        <v>7</v>
-      </c>
-      <c r="C10" s="18">
-        <f t="shared" si="8"/>
-        <v>5</v>
-      </c>
-      <c r="D10" s="19" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="E10" s="8">
+        <v>6</v>
+      </c>
+      <c r="S7" s="9">
         <f t="shared" si="8"/>
         <v>8</v>
       </c>
+      <c r="T7" s="10">
+        <f t="shared" si="9"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="2:20" ht="25.2" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="11">
+        <f t="shared" ref="B8:J8" si="15">IF(B28&lt;&gt;"_", B28, "")</f>
+        <v>6</v>
+      </c>
+      <c r="C8" s="12" t="str">
+        <f t="shared" si="15"/>
+        <v/>
+      </c>
+      <c r="D8" s="13">
+        <f t="shared" si="15"/>
+        <v>3</v>
+      </c>
+      <c r="E8" s="3">
+        <f t="shared" si="15"/>
+        <v>1</v>
+      </c>
+      <c r="F8" s="4" t="str">
+        <f t="shared" si="15"/>
+        <v/>
+      </c>
+      <c r="G8" s="5">
+        <f t="shared" si="15"/>
+        <v>9</v>
+      </c>
+      <c r="H8" s="11" t="str">
+        <f t="shared" si="15"/>
+        <v/>
+      </c>
+      <c r="I8" s="12">
+        <f t="shared" si="15"/>
+        <v>4</v>
+      </c>
+      <c r="J8" s="13" t="str">
+        <f t="shared" si="15"/>
+        <v/>
+      </c>
+      <c r="L8" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="M8" s="12">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="N8" s="13" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="O8" s="3" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="P8" s="4">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="Q8" s="5">
+        <f t="shared" si="6"/>
+        <v>9</v>
+      </c>
+      <c r="R8" s="11" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="S8" s="12" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="T8" s="13" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+    </row>
+    <row r="9" spans="2:20" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="14" t="str">
+        <f t="shared" ref="B9:J9" si="16">IF(B29&lt;&gt;"_", B29, "")</f>
+        <v/>
+      </c>
+      <c r="C9" s="15" t="str">
+        <f t="shared" si="16"/>
+        <v/>
+      </c>
+      <c r="D9" s="16">
+        <f t="shared" si="16"/>
+        <v>5</v>
+      </c>
+      <c r="E9" s="6" t="str">
+        <f t="shared" si="16"/>
+        <v/>
+      </c>
+      <c r="F9" s="2">
+        <f t="shared" si="16"/>
+        <v>7</v>
+      </c>
+      <c r="G9" s="7" t="str">
+        <f t="shared" si="16"/>
+        <v/>
+      </c>
+      <c r="H9" s="14">
+        <f t="shared" si="16"/>
+        <v>3</v>
+      </c>
+      <c r="I9" s="15">
+        <f t="shared" si="16"/>
+        <v>9</v>
+      </c>
+      <c r="J9" s="16" t="str">
+        <f t="shared" si="16"/>
+        <v/>
+      </c>
+      <c r="L9" s="14">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="M9" s="15">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="N9" s="16" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="O9" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="P9" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="Q9" s="7" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="R9" s="14">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="S9" s="15" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="T9" s="16" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+    </row>
+    <row r="10" spans="2:20" ht="25.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B10" s="17" t="str">
+        <f t="shared" ref="B10:J10" si="17">IF(B30&lt;&gt;"_", B30, "")</f>
+        <v/>
+      </c>
+      <c r="C10" s="18" t="str">
+        <f t="shared" si="17"/>
+        <v/>
+      </c>
+      <c r="D10" s="19">
+        <f t="shared" si="17"/>
+        <v>9</v>
+      </c>
+      <c r="E10" s="8" t="str">
+        <f t="shared" si="17"/>
+        <v/>
+      </c>
       <c r="F10" s="9" t="str">
+        <f t="shared" si="17"/>
+        <v/>
+      </c>
+      <c r="G10" s="10" t="str">
+        <f t="shared" si="17"/>
+        <v/>
+      </c>
+      <c r="H10" s="17" t="str">
+        <f t="shared" si="17"/>
+        <v/>
+      </c>
+      <c r="I10" s="18">
+        <f t="shared" si="17"/>
+        <v>6</v>
+      </c>
+      <c r="J10" s="19" t="str">
+        <f t="shared" si="17"/>
+        <v/>
+      </c>
+      <c r="L10" s="17" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="M10" s="18">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="N10" s="19" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="O10" s="8" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="P10" s="9">
+        <f t="shared" si="5"/>
+        <v>7</v>
+      </c>
+      <c r="Q10" s="10">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="R10" s="17" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="S10" s="18" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
-      <c r="G10" s="10">
-        <f t="shared" si="8"/>
-        <v>9</v>
-      </c>
-      <c r="H10" s="17" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="I10" s="18" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="J10" s="19" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="L10" s="17" t="str">
-        <f>IF(B41&lt;&gt;"_",B41, "")</f>
-        <v/>
-      </c>
-      <c r="M10" s="18">
-        <f>IF(C41&lt;&gt;"_",C41, "")</f>
-        <v>2</v>
-      </c>
-      <c r="N10" s="19" t="str">
-        <f>IF(D41&lt;&gt;"_",D41, "")</f>
-        <v/>
-      </c>
-      <c r="O10" s="8" t="str">
-        <f>IF(E41&lt;&gt;"_",E41, "")</f>
-        <v/>
-      </c>
-      <c r="P10" s="9">
-        <f>IF(F41&lt;&gt;"_",F41, "")</f>
-        <v>7</v>
-      </c>
-      <c r="Q10" s="10">
-        <f>IF(G41&lt;&gt;"_",G41, "")</f>
-        <v>1</v>
-      </c>
-      <c r="R10" s="17" t="str">
-        <f>IF(H41&lt;&gt;"_",H41, "")</f>
-        <v/>
-      </c>
-      <c r="S10" s="18" t="str">
-        <f>IF(I41&lt;&gt;"_",I41, "")</f>
-        <v/>
-      </c>
       <c r="T10" s="19">
-        <f>IF(J41&lt;&gt;"_",J41, "")</f>
+        <f t="shared" si="9"/>
         <v>4</v>
       </c>
     </row>
     <row r="11" spans="2:20" ht="78.599999999999994" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="12" spans="2:20" ht="25.2" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B12" s="11">
-        <f>IF(B44&lt;&gt;"_", B44, "")</f>
+        <f t="shared" ref="B12:J12" si="18">IF(B44&lt;&gt;"_", B44, "")</f>
         <v>5</v>
       </c>
       <c r="C12" s="12" t="str">
-        <f>IF(C44&lt;&gt;"_", C44, "")</f>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="D12" s="13">
-        <f>IF(D44&lt;&gt;"_", D44, "")</f>
+        <f t="shared" si="18"/>
         <v>3</v>
       </c>
       <c r="E12" s="3" t="str">
-        <f>IF(E44&lt;&gt;"_", E44, "")</f>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="F12" s="4" t="str">
-        <f>IF(F44&lt;&gt;"_", F44, "")</f>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="G12" s="5" t="str">
-        <f>IF(G44&lt;&gt;"_", G44, "")</f>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="H12" s="11" t="str">
-        <f>IF(H44&lt;&gt;"_", H44, "")</f>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="I12" s="12" t="str">
-        <f>IF(I44&lt;&gt;"_", I44, "")</f>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="J12" s="13" t="str">
-        <f>IF(J44&lt;&gt;"_", J44, "")</f>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="L12" s="11">
-        <f>IF(B55&lt;&gt;"_",B55, "")</f>
+        <f t="shared" ref="L12:L20" si="19">IF(B55&lt;&gt;"_",B55, "")</f>
         <v>5</v>
       </c>
       <c r="M12" s="12" t="str">
-        <f>IF(C55&lt;&gt;"_",C55, "")</f>
+        <f t="shared" ref="M12:M20" si="20">IF(C55&lt;&gt;"_",C55, "")</f>
         <v/>
       </c>
       <c r="N12" s="13" t="str">
-        <f>IF(D55&lt;&gt;"_",D55, "")</f>
+        <f t="shared" ref="N12:N20" si="21">IF(D55&lt;&gt;"_",D55, "")</f>
         <v/>
       </c>
       <c r="O12" s="3">
-        <f>IF(E55&lt;&gt;"_",E55, "")</f>
+        <f t="shared" ref="O12:O20" si="22">IF(E55&lt;&gt;"_",E55, "")</f>
         <v>9</v>
       </c>
       <c r="P12" s="4" t="str">
-        <f>IF(F55&lt;&gt;"_",F55, "")</f>
+        <f t="shared" ref="P12:P20" si="23">IF(F55&lt;&gt;"_",F55, "")</f>
         <v/>
       </c>
       <c r="Q12" s="5" t="str">
-        <f>IF(G55&lt;&gt;"_",G55, "")</f>
+        <f t="shared" ref="Q12:Q20" si="24">IF(G55&lt;&gt;"_",G55, "")</f>
         <v/>
       </c>
       <c r="R12" s="11" t="str">
-        <f>IF(H55&lt;&gt;"_",H55, "")</f>
+        <f t="shared" ref="R12:R20" si="25">IF(H55&lt;&gt;"_",H55, "")</f>
         <v/>
       </c>
       <c r="S12" s="12">
-        <f>IF(I55&lt;&gt;"_",I55, "")</f>
+        <f t="shared" ref="S12:S20" si="26">IF(I55&lt;&gt;"_",I55, "")</f>
         <v>4</v>
       </c>
       <c r="T12" s="13" t="str">
-        <f>IF(J55&lt;&gt;"_",J55, "")</f>
+        <f t="shared" ref="T12:T20" si="27">IF(J55&lt;&gt;"_",J55, "")</f>
         <v/>
       </c>
     </row>
     <row r="13" spans="2:20" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="14" t="str">
-        <f>IF(B45&lt;&gt;"_", B45, "")</f>
+        <f t="shared" ref="B13:J13" si="28">IF(B45&lt;&gt;"_", B45, "")</f>
         <v/>
       </c>
       <c r="C13" s="15" t="str">
-        <f>IF(C45&lt;&gt;"_", C45, "")</f>
+        <f t="shared" si="28"/>
         <v/>
       </c>
       <c r="D13" s="16">
-        <f>IF(D45&lt;&gt;"_", D45, "")</f>
+        <f t="shared" si="28"/>
         <v>4</v>
       </c>
       <c r="E13" s="6" t="str">
-        <f>IF(E45&lt;&gt;"_", E45, "")</f>
+        <f t="shared" si="28"/>
         <v/>
       </c>
       <c r="F13" s="2">
-        <f>IF(F45&lt;&gt;"_", F45, "")</f>
+        <f t="shared" si="28"/>
         <v>5</v>
       </c>
       <c r="G13" s="7">
-        <f>IF(G45&lt;&gt;"_", G45, "")</f>
+        <f t="shared" si="28"/>
         <v>2</v>
       </c>
       <c r="H13" s="14">
-        <f>IF(H45&lt;&gt;"_", H45, "")</f>
+        <f t="shared" si="28"/>
         <v>3</v>
       </c>
       <c r="I13" s="15" t="str">
-        <f>IF(I45&lt;&gt;"_", I45, "")</f>
+        <f t="shared" si="28"/>
         <v/>
       </c>
       <c r="J13" s="16" t="str">
-        <f>IF(J45&lt;&gt;"_", J45, "")</f>
+        <f t="shared" si="28"/>
         <v/>
       </c>
       <c r="L13" s="14">
-        <f>IF(B56&lt;&gt;"_",B56, "")</f>
+        <f t="shared" si="19"/>
         <v>3</v>
       </c>
       <c r="M13" s="15" t="str">
-        <f>IF(C56&lt;&gt;"_",C56, "")</f>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="N13" s="16" t="str">
-        <f>IF(D56&lt;&gt;"_",D56, "")</f>
+        <f t="shared" si="21"/>
         <v/>
       </c>
       <c r="O13" s="6" t="str">
-        <f>IF(E56&lt;&gt;"_",E56, "")</f>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="P13" s="2">
-        <f>IF(F56&lt;&gt;"_",F56, "")</f>
+        <f t="shared" si="23"/>
         <v>7</v>
       </c>
       <c r="Q13" s="7" t="str">
-        <f>IF(G56&lt;&gt;"_",G56, "")</f>
+        <f t="shared" si="24"/>
         <v/>
       </c>
       <c r="R13" s="14">
-        <f>IF(H56&lt;&gt;"_",H56, "")</f>
+        <f t="shared" si="25"/>
         <v>9</v>
       </c>
       <c r="S13" s="15">
-        <f>IF(I56&lt;&gt;"_",I56, "")</f>
+        <f t="shared" si="26"/>
         <v>2</v>
       </c>
       <c r="T13" s="16">
-        <f>IF(J56&lt;&gt;"_",J56, "")</f>
+        <f t="shared" si="27"/>
         <v>5</v>
       </c>
     </row>
     <row r="14" spans="2:20" ht="25.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B14" s="17">
-        <f>IF(B46&lt;&gt;"_", B46, "")</f>
+        <f t="shared" ref="B14:J14" si="29">IF(B46&lt;&gt;"_", B46, "")</f>
         <v>1</v>
       </c>
       <c r="C14" s="18" t="str">
-        <f>IF(C46&lt;&gt;"_", C46, "")</f>
+        <f t="shared" si="29"/>
         <v/>
       </c>
       <c r="D14" s="19" t="str">
-        <f>IF(D46&lt;&gt;"_", D46, "")</f>
+        <f t="shared" si="29"/>
         <v/>
       </c>
       <c r="E14" s="8" t="str">
-        <f>IF(E46&lt;&gt;"_", E46, "")</f>
+        <f t="shared" si="29"/>
         <v/>
       </c>
       <c r="F14" s="9">
-        <f>IF(F46&lt;&gt;"_", F46, "")</f>
+        <f t="shared" si="29"/>
         <v>7</v>
       </c>
       <c r="G14" s="10">
-        <f>IF(G46&lt;&gt;"_", G46, "")</f>
+        <f t="shared" si="29"/>
         <v>9</v>
       </c>
       <c r="H14" s="17" t="str">
-        <f>IF(H46&lt;&gt;"_", H46, "")</f>
+        <f t="shared" si="29"/>
         <v/>
       </c>
       <c r="I14" s="18">
-        <f>IF(I46&lt;&gt;"_", I46, "")</f>
+        <f t="shared" si="29"/>
         <v>4</v>
       </c>
       <c r="J14" s="19" t="str">
-        <f>IF(J46&lt;&gt;"_", J46, "")</f>
+        <f t="shared" si="29"/>
         <v/>
       </c>
       <c r="L14" s="17">
-        <f>IF(B57&lt;&gt;"_",B57, "")</f>
+        <f t="shared" si="19"/>
         <v>6</v>
       </c>
       <c r="M14" s="18">
-        <f>IF(C57&lt;&gt;"_",C57, "")</f>
+        <f t="shared" si="20"/>
         <v>9</v>
       </c>
       <c r="N14" s="19" t="str">
-        <f>IF(D57&lt;&gt;"_",D57, "")</f>
+        <f t="shared" si="21"/>
         <v/>
       </c>
       <c r="O14" s="8" t="str">
-        <f>IF(E57&lt;&gt;"_",E57, "")</f>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="P14" s="9">
-        <f>IF(F57&lt;&gt;"_",F57, "")</f>
+        <f t="shared" si="23"/>
         <v>2</v>
       </c>
       <c r="Q14" s="10" t="str">
-        <f>IF(G57&lt;&gt;"_",G57, "")</f>
+        <f t="shared" si="24"/>
         <v/>
       </c>
       <c r="R14" s="17" t="str">
-        <f>IF(H57&lt;&gt;"_",H57, "")</f>
+        <f t="shared" si="25"/>
         <v/>
       </c>
       <c r="S14" s="18" t="str">
-        <f>IF(I57&lt;&gt;"_",I57, "")</f>
+        <f t="shared" si="26"/>
         <v/>
       </c>
       <c r="T14" s="19" t="str">
-        <f>IF(J57&lt;&gt;"_",J57, "")</f>
+        <f t="shared" si="27"/>
         <v/>
       </c>
     </row>
     <row r="15" spans="2:20" ht="25.2" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B15" s="3">
-        <f>IF(B47&lt;&gt;"_", B47, "")</f>
+        <f t="shared" ref="B15:J15" si="30">IF(B47&lt;&gt;"_", B47, "")</f>
         <v>2</v>
       </c>
       <c r="C15" s="4" t="str">
-        <f>IF(C47&lt;&gt;"_", C47, "")</f>
+        <f t="shared" si="30"/>
         <v/>
       </c>
       <c r="D15" s="5" t="str">
-        <f>IF(D47&lt;&gt;"_", D47, "")</f>
+        <f t="shared" si="30"/>
         <v/>
       </c>
       <c r="E15" s="11">
-        <f>IF(E47&lt;&gt;"_", E47, "")</f>
+        <f t="shared" si="30"/>
         <v>7</v>
       </c>
       <c r="F15" s="12" t="str">
-        <f>IF(F47&lt;&gt;"_", F47, "")</f>
+        <f t="shared" si="30"/>
         <v/>
       </c>
       <c r="G15" s="13" t="str">
-        <f>IF(G47&lt;&gt;"_", G47, "")</f>
+        <f t="shared" si="30"/>
         <v/>
       </c>
       <c r="H15" s="3" t="str">
-        <f>IF(H47&lt;&gt;"_", H47, "")</f>
+        <f t="shared" si="30"/>
         <v/>
       </c>
       <c r="I15" s="4">
-        <f>IF(I47&lt;&gt;"_", I47, "")</f>
+        <f t="shared" si="30"/>
         <v>3</v>
       </c>
       <c r="J15" s="5">
-        <f>IF(J47&lt;&gt;"_", J47, "")</f>
+        <f t="shared" si="30"/>
         <v>4</v>
       </c>
       <c r="L15" s="3">
-        <f>IF(B58&lt;&gt;"_",B58, "")</f>
+        <f t="shared" si="19"/>
         <v>7</v>
       </c>
       <c r="M15" s="4" t="str">
-        <f>IF(C58&lt;&gt;"_",C58, "")</f>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="N15" s="5">
-        <f>IF(D58&lt;&gt;"_",D58, "")</f>
+        <f t="shared" si="21"/>
         <v>3</v>
       </c>
       <c r="O15" s="11" t="str">
-        <f>IF(E58&lt;&gt;"_",E58, "")</f>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="P15" s="12" t="str">
-        <f>IF(F58&lt;&gt;"_",F58, "")</f>
+        <f t="shared" si="23"/>
         <v/>
       </c>
       <c r="Q15" s="13" t="str">
-        <f>IF(G58&lt;&gt;"_",G58, "")</f>
+        <f t="shared" si="24"/>
         <v/>
       </c>
       <c r="R15" s="3" t="str">
-        <f>IF(H58&lt;&gt;"_",H58, "")</f>
+        <f t="shared" si="25"/>
         <v/>
       </c>
       <c r="S15" s="4" t="str">
-        <f>IF(I58&lt;&gt;"_",I58, "")</f>
+        <f t="shared" si="26"/>
         <v/>
       </c>
       <c r="T15" s="5" t="str">
-        <f>IF(J58&lt;&gt;"_",J58, "")</f>
+        <f t="shared" si="27"/>
         <v/>
       </c>
     </row>
     <row r="16" spans="2:20" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="6" t="str">
-        <f>IF(B48&lt;&gt;"_", B48, "")</f>
+        <f t="shared" ref="B16:J16" si="31">IF(B48&lt;&gt;"_", B48, "")</f>
         <v/>
       </c>
       <c r="C16" s="2" t="str">
-        <f>IF(C48&lt;&gt;"_", C48, "")</f>
+        <f t="shared" si="31"/>
         <v/>
       </c>
       <c r="D16" s="7" t="str">
-        <f>IF(D48&lt;&gt;"_", D48, "")</f>
+        <f t="shared" si="31"/>
         <v/>
       </c>
       <c r="E16" s="14">
-        <f>IF(E48&lt;&gt;"_", E48, "")</f>
+        <f t="shared" si="31"/>
         <v>2</v>
       </c>
       <c r="F16" s="15" t="str">
-        <f>IF(F48&lt;&gt;"_", F48, "")</f>
+        <f t="shared" si="31"/>
         <v/>
       </c>
       <c r="G16" s="16">
-        <f>IF(G48&lt;&gt;"_", G48, "")</f>
+        <f t="shared" si="31"/>
         <v>6</v>
       </c>
       <c r="H16" s="6" t="str">
-        <f>IF(H48&lt;&gt;"_", H48, "")</f>
+        <f t="shared" si="31"/>
         <v/>
       </c>
       <c r="I16" s="2" t="str">
-        <f>IF(I48&lt;&gt;"_", I48, "")</f>
+        <f t="shared" si="31"/>
         <v/>
       </c>
       <c r="J16" s="7">
-        <f>IF(J48&lt;&gt;"_", J48, "")</f>
+        <f t="shared" si="31"/>
         <v>5</v>
       </c>
       <c r="L16" s="6" t="str">
-        <f>IF(B59&lt;&gt;"_",B59, "")</f>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="M16" s="2" t="str">
-        <f>IF(C59&lt;&gt;"_",C59, "")</f>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="N16" s="7">
-        <f>IF(D59&lt;&gt;"_",D59, "")</f>
+        <f t="shared" si="21"/>
         <v>9</v>
       </c>
       <c r="O16" s="14" t="str">
-        <f>IF(E59&lt;&gt;"_",E59, "")</f>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="P16" s="15">
-        <f>IF(F59&lt;&gt;"_",F59, "")</f>
+        <f t="shared" si="23"/>
         <v>5</v>
       </c>
       <c r="Q16" s="16" t="str">
-        <f>IF(G59&lt;&gt;"_",G59, "")</f>
+        <f t="shared" si="24"/>
         <v/>
       </c>
       <c r="R16" s="6">
-        <f>IF(H59&lt;&gt;"_",H59, "")</f>
+        <f t="shared" si="25"/>
         <v>4</v>
       </c>
       <c r="S16" s="2" t="str">
-        <f>IF(I59&lt;&gt;"_",I59, "")</f>
+        <f t="shared" si="26"/>
         <v/>
       </c>
       <c r="T16" s="7">
-        <f>IF(J59&lt;&gt;"_",J59, "")</f>
+        <f t="shared" si="27"/>
         <v>3</v>
       </c>
     </row>
     <row r="17" spans="2:20" ht="25.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B17" s="8">
-        <f>IF(B49&lt;&gt;"_", B49, "")</f>
+        <f t="shared" ref="B17:J17" si="32">IF(B49&lt;&gt;"_", B49, "")</f>
         <v>4</v>
       </c>
       <c r="C17" s="9">
-        <f>IF(C49&lt;&gt;"_", C49, "")</f>
+        <f t="shared" si="32"/>
         <v>1</v>
       </c>
       <c r="D17" s="10">
-        <f>IF(D49&lt;&gt;"_", D49, "")</f>
+        <f t="shared" si="32"/>
         <v>7</v>
       </c>
       <c r="E17" s="17">
-        <f>IF(E49&lt;&gt;"_", E49, "")</f>
+        <f t="shared" si="32"/>
         <v>5</v>
       </c>
       <c r="F17" s="18" t="str">
-        <f>IF(F49&lt;&gt;"_", F49, "")</f>
+        <f t="shared" si="32"/>
         <v/>
       </c>
       <c r="G17" s="19" t="str">
-        <f>IF(G49&lt;&gt;"_", G49, "")</f>
+        <f t="shared" si="32"/>
         <v/>
       </c>
       <c r="H17" s="8" t="str">
-        <f>IF(H49&lt;&gt;"_", H49, "")</f>
+        <f t="shared" si="32"/>
         <v/>
       </c>
       <c r="I17" s="9" t="str">
-        <f>IF(I49&lt;&gt;"_", I49, "")</f>
+        <f t="shared" si="32"/>
         <v/>
       </c>
       <c r="J17" s="10">
-        <f>IF(J49&lt;&gt;"_", J49, "")</f>
+        <f t="shared" si="32"/>
         <v>6</v>
       </c>
       <c r="L17" s="8" t="str">
-        <f>IF(B60&lt;&gt;"_",B60, "")</f>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="M17" s="9">
-        <f>IF(C60&lt;&gt;"_",C60, "")</f>
+        <f t="shared" si="20"/>
         <v>4</v>
       </c>
       <c r="N17" s="10" t="str">
-        <f>IF(D60&lt;&gt;"_",D60, "")</f>
+        <f t="shared" si="21"/>
         <v/>
       </c>
       <c r="O17" s="17">
-        <f>IF(E60&lt;&gt;"_",E60, "")</f>
+        <f t="shared" si="22"/>
         <v>7</v>
       </c>
       <c r="P17" s="18">
-        <f>IF(F60&lt;&gt;"_",F60, "")</f>
+        <f t="shared" si="23"/>
         <v>1</v>
       </c>
       <c r="Q17" s="19">
-        <f>IF(G60&lt;&gt;"_",G60, "")</f>
+        <f t="shared" si="24"/>
         <v>3</v>
       </c>
       <c r="R17" s="8">
-        <f>IF(H60&lt;&gt;"_",H60, "")</f>
+        <f t="shared" si="25"/>
         <v>6</v>
       </c>
       <c r="S17" s="9">
-        <f>IF(I60&lt;&gt;"_",I60, "")</f>
+        <f t="shared" si="26"/>
         <v>5</v>
       </c>
       <c r="T17" s="10" t="str">
-        <f>IF(J60&lt;&gt;"_",J60, "")</f>
+        <f t="shared" si="27"/>
         <v/>
       </c>
     </row>
     <row r="18" spans="2:20" ht="25.2" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B18" s="11" t="str">
-        <f>IF(B50&lt;&gt;"_", B50, "")</f>
+        <f t="shared" ref="B18:J18" si="33">IF(B50&lt;&gt;"_", B50, "")</f>
         <v/>
       </c>
       <c r="C18" s="12" t="str">
-        <f>IF(C50&lt;&gt;"_", C50, "")</f>
+        <f t="shared" si="33"/>
         <v/>
       </c>
       <c r="D18" s="13">
-        <f>IF(D50&lt;&gt;"_", D50, "")</f>
+        <f t="shared" si="33"/>
         <v>1</v>
       </c>
       <c r="E18" s="3">
-        <f>IF(E50&lt;&gt;"_", E50, "")</f>
+        <f t="shared" si="33"/>
         <v>6</v>
       </c>
       <c r="F18" s="4" t="str">
-        <f>IF(F50&lt;&gt;"_", F50, "")</f>
+        <f t="shared" si="33"/>
         <v/>
       </c>
       <c r="G18" s="5" t="str">
-        <f>IF(G50&lt;&gt;"_", G50, "")</f>
+        <f t="shared" si="33"/>
         <v/>
       </c>
       <c r="H18" s="11" t="str">
-        <f>IF(H50&lt;&gt;"_", H50, "")</f>
+        <f t="shared" si="33"/>
         <v/>
       </c>
       <c r="I18" s="12" t="str">
-        <f>IF(I50&lt;&gt;"_", I50, "")</f>
+        <f t="shared" si="33"/>
         <v/>
       </c>
       <c r="J18" s="13">
-        <f>IF(J50&lt;&gt;"_", J50, "")</f>
+        <f t="shared" si="33"/>
         <v>2</v>
       </c>
       <c r="L18" s="11" t="str">
-        <f>IF(B61&lt;&gt;"_",B61, "")</f>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="M18" s="12">
-        <f>IF(C61&lt;&gt;"_",C61, "")</f>
+        <f t="shared" si="20"/>
         <v>2</v>
       </c>
       <c r="N18" s="13">
-        <f>IF(D61&lt;&gt;"_",D61, "")</f>
+        <f t="shared" si="21"/>
         <v>6</v>
       </c>
       <c r="O18" s="3" t="str">
-        <f>IF(E61&lt;&gt;"_",E61, "")</f>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="P18" s="4" t="str">
-        <f>IF(F61&lt;&gt;"_",F61, "")</f>
+        <f t="shared" si="23"/>
         <v/>
       </c>
       <c r="Q18" s="5">
-        <f>IF(G61&lt;&gt;"_",G61, "")</f>
+        <f t="shared" si="24"/>
         <v>7</v>
       </c>
       <c r="R18" s="11" t="str">
-        <f>IF(H61&lt;&gt;"_",H61, "")</f>
+        <f t="shared" si="25"/>
         <v/>
       </c>
       <c r="S18" s="12">
-        <f>IF(I61&lt;&gt;"_",I61, "")</f>
+        <f t="shared" si="26"/>
         <v>1</v>
       </c>
       <c r="T18" s="13" t="str">
-        <f>IF(J61&lt;&gt;"_",J61, "")</f>
+        <f t="shared" si="27"/>
         <v/>
       </c>
     </row>
     <row r="19" spans="2:20" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="14">
-        <f>IF(B51&lt;&gt;"_", B51, "")</f>
+        <f t="shared" ref="B19:J19" si="34">IF(B51&lt;&gt;"_", B51, "")</f>
         <v>8</v>
       </c>
       <c r="C19" s="15">
-        <f>IF(C51&lt;&gt;"_", C51, "")</f>
+        <f t="shared" si="34"/>
         <v>4</v>
       </c>
       <c r="D19" s="16" t="str">
-        <f>IF(D51&lt;&gt;"_", D51, "")</f>
+        <f t="shared" si="34"/>
         <v/>
       </c>
       <c r="E19" s="6" t="str">
-        <f>IF(E51&lt;&gt;"_", E51, "")</f>
+        <f t="shared" si="34"/>
         <v/>
       </c>
       <c r="F19" s="2">
-        <f>IF(F51&lt;&gt;"_", F51, "")</f>
+        <f t="shared" si="34"/>
         <v>3</v>
       </c>
       <c r="G19" s="7">
-        <f>IF(G51&lt;&gt;"_", G51, "")</f>
+        <f t="shared" si="34"/>
         <v>1</v>
       </c>
       <c r="H19" s="14" t="str">
-        <f>IF(H51&lt;&gt;"_", H51, "")</f>
+        <f t="shared" si="34"/>
         <v/>
       </c>
       <c r="I19" s="15">
-        <f>IF(I51&lt;&gt;"_", I51, "")</f>
+        <f t="shared" si="34"/>
         <v>5</v>
       </c>
       <c r="J19" s="16">
-        <f>IF(J51&lt;&gt;"_", J51, "")</f>
+        <f t="shared" si="34"/>
         <v>7</v>
       </c>
       <c r="L19" s="14" t="str">
-        <f>IF(B62&lt;&gt;"_",B62, "")</f>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="M19" s="15">
-        <f>IF(C62&lt;&gt;"_",C62, "")</f>
+        <f t="shared" si="20"/>
         <v>7</v>
       </c>
       <c r="N19" s="16">
-        <f>IF(D62&lt;&gt;"_",D62, "")</f>
+        <f t="shared" si="21"/>
         <v>5</v>
       </c>
       <c r="O19" s="6" t="str">
-        <f>IF(E62&lt;&gt;"_",E62, "")</f>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="P19" s="2">
-        <f>IF(F62&lt;&gt;"_",F62, "")</f>
+        <f t="shared" si="23"/>
         <v>6</v>
       </c>
       <c r="Q19" s="7" t="str">
-        <f>IF(G62&lt;&gt;"_",G62, "")</f>
+        <f t="shared" si="24"/>
         <v/>
       </c>
       <c r="R19" s="14" t="str">
-        <f>IF(H62&lt;&gt;"_",H62, "")</f>
+        <f t="shared" si="25"/>
         <v/>
       </c>
       <c r="S19" s="15" t="str">
-        <f>IF(I62&lt;&gt;"_",I62, "")</f>
+        <f t="shared" si="26"/>
         <v/>
       </c>
       <c r="T19" s="16">
-        <f>IF(J62&lt;&gt;"_",J62, "")</f>
+        <f t="shared" si="27"/>
         <v>8</v>
       </c>
     </row>
     <row r="20" spans="2:20" ht="25.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B20" s="17">
-        <f>IF(B52&lt;&gt;"_", B52, "")</f>
+        <f t="shared" ref="B20:J20" si="35">IF(B52&lt;&gt;"_", B52, "")</f>
         <v>6</v>
       </c>
       <c r="C20" s="18" t="str">
-        <f>IF(C52&lt;&gt;"_", C52, "")</f>
+        <f t="shared" si="35"/>
         <v/>
       </c>
       <c r="D20" s="19" t="str">
-        <f>IF(D52&lt;&gt;"_", D52, "")</f>
+        <f t="shared" si="35"/>
         <v/>
       </c>
       <c r="E20" s="8" t="str">
-        <f>IF(E52&lt;&gt;"_", E52, "")</f>
+        <f t="shared" si="35"/>
         <v/>
       </c>
       <c r="F20" s="9">
-        <f>IF(F52&lt;&gt;"_", F52, "")</f>
+        <f t="shared" si="35"/>
         <v>2</v>
       </c>
       <c r="G20" s="10" t="str">
-        <f>IF(G52&lt;&gt;"_", G52, "")</f>
+        <f t="shared" si="35"/>
         <v/>
       </c>
       <c r="H20" s="17">
-        <f>IF(H52&lt;&gt;"_", H52, "")</f>
+        <f t="shared" si="35"/>
         <v>1</v>
       </c>
       <c r="I20" s="18" t="str">
-        <f>IF(I52&lt;&gt;"_", I52, "")</f>
+        <f t="shared" si="35"/>
         <v/>
       </c>
       <c r="J20" s="19" t="str">
-        <f>IF(J52&lt;&gt;"_", J52, "")</f>
+        <f t="shared" si="35"/>
         <v/>
       </c>
       <c r="L20" s="17" t="str">
-        <f>IF(B63&lt;&gt;"_",B63, "")</f>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="M20" s="18" t="str">
-        <f>IF(C63&lt;&gt;"_",C63, "")</f>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="N20" s="19" t="str">
-        <f>IF(D63&lt;&gt;"_",D63, "")</f>
+        <f t="shared" si="21"/>
         <v/>
       </c>
       <c r="O20" s="8">
-        <f>IF(E63&lt;&gt;"_",E63, "")</f>
+        <f t="shared" si="22"/>
         <v>2</v>
       </c>
       <c r="P20" s="9">
-        <f>IF(F63&lt;&gt;"_",F63, "")</f>
+        <f t="shared" si="23"/>
         <v>8</v>
       </c>
       <c r="Q20" s="10" t="str">
-        <f>IF(G63&lt;&gt;"_",G63, "")</f>
+        <f t="shared" si="24"/>
         <v/>
       </c>
       <c r="R20" s="17" t="str">
-        <f>IF(H63&lt;&gt;"_",H63, "")</f>
+        <f t="shared" si="25"/>
         <v/>
       </c>
       <c r="S20" s="18">
-        <f>IF(I63&lt;&gt;"_",I63, "")</f>
+        <f t="shared" si="26"/>
         <v>6</v>
       </c>
       <c r="T20" s="19" t="str">
-        <f>IF(J63&lt;&gt;"_",J63, "")</f>
+        <f t="shared" si="27"/>
         <v/>
       </c>
     </row>
@@ -1952,20 +1952,20 @@
       <c r="D22" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E22" s="1">
+      <c r="E22" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F22" s="1">
         <v>4</v>
       </c>
-      <c r="F22" s="1">
-        <v>6</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>0</v>
+      <c r="G22" s="1">
+        <v>1</v>
+      </c>
+      <c r="H22" s="1">
+        <v>5</v>
       </c>
       <c r="I22" s="1">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="J22" s="1" t="s">
         <v>0</v>
@@ -1975,8 +1975,8 @@
       <c r="B23" s="1">
         <v>3</v>
       </c>
-      <c r="C23" s="1" t="s">
-        <v>0</v>
+      <c r="C23" s="1">
+        <v>5</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>0</v>
@@ -1984,14 +1984,14 @@
       <c r="E23" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F23" s="1">
-        <v>5</v>
+      <c r="F23" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="G23" s="1" t="s">
         <v>0</v>
       </c>
       <c r="H23" s="1">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="I23" s="1" t="s">
         <v>0</v>
@@ -2001,49 +2001,49 @@
       </c>
     </row>
     <row r="24" spans="2:20" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="1">
-        <v>8</v>
+      <c r="B24" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D24" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>0</v>
       </c>
       <c r="F24" s="1">
-        <v>7</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="H24" s="1">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="G24" s="1">
+        <v>6</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="I24" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="J24" s="1" t="s">
-        <v>0</v>
+      <c r="J24" s="1">
+        <v>2</v>
       </c>
     </row>
     <row r="25" spans="2:20" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="1">
+        <v>4</v>
+      </c>
+      <c r="C25" s="1">
+        <v>2</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E25" s="1">
         <v>9</v>
       </c>
-      <c r="C25" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D25" s="1">
-        <v>1</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>0</v>
+      <c r="F25" s="1">
+        <v>1</v>
       </c>
       <c r="G25" s="1" t="s">
         <v>0</v>
@@ -2052,7 +2052,7 @@
         <v>0</v>
       </c>
       <c r="I25" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J25" s="1" t="s">
         <v>0</v>
@@ -2060,7 +2060,7 @@
     </row>
     <row r="26" spans="2:20" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>0</v>
@@ -2068,23 +2068,23 @@
       <c r="D26" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E26" s="1">
-        <v>3</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>0</v>
+      <c r="E26" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F26" s="1">
+        <v>6</v>
       </c>
       <c r="G26" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="H26" s="1" t="s">
-        <v>0</v>
+      <c r="H26" s="1">
+        <v>8</v>
       </c>
       <c r="I26" s="1">
-        <v>5</v>
-      </c>
-      <c r="J26" s="1">
-        <v>7</v>
+        <v>1</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="2:20" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2095,109 +2095,109 @@
         <v>0</v>
       </c>
       <c r="D27" s="1">
-        <v>5</v>
-      </c>
-      <c r="E27" s="1">
-        <v>6</v>
-      </c>
-      <c r="F27" s="1">
-        <v>8</v>
+        <v>1</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="G27" s="1">
+        <v>5</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I27" s="1">
+        <v>2</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="2:20" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="1">
+        <v>6</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D28" s="1">
+        <v>3</v>
+      </c>
+      <c r="E28" s="1">
+        <v>1</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G28" s="1">
+        <v>9</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I28" s="1">
         <v>4</v>
       </c>
-      <c r="H27" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="I27" s="1">
-        <v>1</v>
-      </c>
-      <c r="J27" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="2:20" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="G28" s="1">
+      <c r="J28" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="2:20" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D29" s="1">
+        <v>5</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F29" s="1">
         <v>7</v>
       </c>
-      <c r="H28" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="I28" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="J28" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="29" spans="2:20" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="1">
-        <v>4</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D29" s="1">
+      <c r="G29" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H29" s="1">
+        <v>3</v>
+      </c>
+      <c r="I29" s="1">
         <v>9</v>
       </c>
-      <c r="E29" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F29" s="1">
-        <v>3</v>
-      </c>
-      <c r="G29" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="H29" s="1">
-        <v>5</v>
-      </c>
-      <c r="I29" s="1">
-        <v>7</v>
-      </c>
-      <c r="J29" s="1">
-        <v>1</v>
+      <c r="J29" s="1" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="2:20" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="1">
-        <v>7</v>
-      </c>
-      <c r="C30" s="1">
-        <v>5</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E30" s="1">
-        <v>8</v>
+      <c r="B30" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D30" s="1">
+        <v>9</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="F30" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="G30" s="1">
-        <v>9</v>
+      <c r="G30" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="H30" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="I30" s="1" t="s">
-        <v>0</v>
+      <c r="I30" s="1">
+        <v>6</v>
       </c>
       <c r="J30" s="1" t="s">
         <v>0</v>

</xml_diff>